<commit_message>
V2 - Added tasks         - Clear Recycle bin daily around 6 PM         - Add in check for AOB to look for 'People V. Wende' Brief
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF1E898-B238-4048-BCA5-418DCF99F0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD98752-C022-40A6-86BC-46990D008DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>ActionCenterCatalog</t>
+  </si>
+  <si>
+    <t>ExcludedTextPatterns</t>
+  </si>
+  <si>
+    <t>People V. Wende</t>
   </si>
 </sst>
 </file>
@@ -748,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1122,8 +1128,12 @@
       <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
       <c r="A51" s="5"/>

</xml_diff>

<commit_message>
V5 - Added Create form task      - Added document missing logic as business exception
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD98752-C022-40A6-86BC-46990D008DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA3B26A-F7AB-437D-BA24-5DB6A34F90F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>Headers</t>
-  </si>
-  <si>
-    <t>Certificate of Compliance,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count@Statement of Appealability@Table of Contents,Topical Index@Table of Authorities@Statement of Facts,Statement of the Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments</t>
   </si>
   <si>
     <t>LaunchOnbase_Prod</t>
@@ -300,9 +297,6 @@
     <t>SystemExcpetion_EmailFrom</t>
   </si>
   <si>
-    <t>3DC-ITQuestions@jud.ca.gov</t>
-  </si>
-  <si>
     <t>SystemExcpetion_EmailCC</t>
   </si>
   <si>
@@ -361,6 +355,9 @@
   </si>
   <si>
     <t>People V. Wende</t>
+  </si>
+  <si>
+    <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count@Statement of Appealability@Table of Contents,Topical Index@Table of Authorities@Statement of Facts,Statement of the Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments</t>
   </si>
 </sst>
 </file>
@@ -754,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:B50"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -805,7 +802,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -816,7 +813,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -837,10 +834,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -858,7 +855,7 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -871,10 +868,10 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
         <v>64</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -882,160 +879,158 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
         <v>70</v>
-      </c>
-      <c r="B15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
         <v>61</v>
       </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
       <c r="B17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="101.5">
+      <c r="A24" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="101.5">
-      <c r="A24" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="B24" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.5">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" ht="14.5">
+    <row r="26" spans="1:3" ht="14.5">
       <c r="A26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.5">
+      <c r="A27" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="14.5">
-      <c r="A27" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.5">
+    <row r="28" spans="1:3" ht="14.5">
       <c r="A28" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:2" ht="14.5">
+    <row r="29" spans="1:3" ht="14.5">
       <c r="A29" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="130.5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="130.5">
       <c r="A30" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="14.5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.5">
       <c r="A31" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="14.5">
+    </row>
+    <row r="32" spans="1:3" ht="14.5">
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="87">
       <c r="A33" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.5">
       <c r="A34" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="14.5">
       <c r="A35" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.5">
       <c r="A36" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>46</v>
@@ -1043,16 +1038,16 @@
     </row>
     <row r="37" spans="1:3" ht="14.5">
       <c r="A37" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="14.5">
       <c r="A38" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
@@ -1072,7 +1067,7 @@
         <v>54</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
@@ -1080,7 +1075,7 @@
         <v>55</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
@@ -1089,18 +1084,18 @@
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
@@ -1109,18 +1104,18 @@
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
@@ -1129,10 +1124,10 @@
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
V6 - Updated the code with New interface for the code filing. - Updated the Stamp date external task after completion of Accept filing.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA3B26A-F7AB-437D-BA24-5DB6A34F90F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5F3231-A009-4923-B723-754F4F6C6BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,7 +357,7 @@
     <t>People V. Wende</t>
   </si>
   <si>
-    <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count@Statement of Appealability@Table of Contents,Topical Index@Table of Authorities@Statement of Facts,Statement of the Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments</t>
+    <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count,Declaration Regarding Word Count,Statement of Word Count@Statement of Appealability@Table of Contents,Topical Index@Table of Authorities,Table of Authority,Table of Cases and Authorities@Statement of Facts,Statement of the Facts,Statement of the Case,Summary of Alleged Facts,Statements of Case and Procedural Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments</t>
   </si>
 </sst>
 </file>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Delgadillo doc is added and with other changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABC4546-60DB-4754-864D-FA845EAD4DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B6FA81-B824-4494-AAC8-9D77F5C8824A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -342,12 +342,6 @@
     <t>ActionCenterCatalog</t>
   </si>
   <si>
-    <t>ExcludedTextPatterns</t>
-  </si>
-  <si>
-    <t>BRIEF - APPELLANT'S OPENING BRIEF;BRIEF - WENDE BRIEF</t>
-  </si>
-  <si>
     <t>AOB_Citations</t>
   </si>
   <si>
@@ -367,6 +361,27 @@
   </si>
   <si>
     <t>People v. Delgadillo</t>
+  </si>
+  <si>
+    <t>AOB_ExcludedTextPatterns</t>
+  </si>
+  <si>
+    <t>Wende_ExcludedTextPatterns</t>
+  </si>
+  <si>
+    <t>People V. Wende,People v. Delgadillo</t>
+  </si>
+  <si>
+    <t>Delgadillo_Citations</t>
+  </si>
+  <si>
+    <t>Delgadillo_Headers</t>
+  </si>
+  <si>
+    <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count,Declaration Regarding Word Count,Statement of Word Count,Certification of Compliance@Statement of Appealability@Table of Contents,Topical Index@Table of Authorities,Table of Authority,Table of Cases and Authorities@Statement of Facts,Statement of the Facts,Statement of the Case,Summary of Alleged Facts,Statements of Case and Procedural Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments@Declaration of Appellate Counsel,Declaration of Counsel,DECLARATION OF,COUNSEL DECLARATION,Certification of Appellate Counsel,Certificate of Appellate Counsel,Attest of Appellate Counsel,Attestation of Appellate Counsel@court may treat the appeal as abandoned and dismiss the appeal,court may dismiss the appeal without issuing an opinion,may result in the court dismissing the appeal as abandoned,the appeal may be dismissed as abandoned,court very likely would dismiss the appeal as abandoned,no brief or letter is filed the appeal may be dismissed,court may treat the appeal as abandoned and dismiss,the court may dismiss the matter,the Court may dismiss the appeal as abandoned,if the appeal is dismissed as abandoned</t>
+  </si>
+  <si>
+    <t>BRIEF - APPELLANT'S OPENING BRIEF;BRIEF - WENDE BRIEF;BRIEF - DELGADILLO BRIEF</t>
   </si>
 </sst>
 </file>
@@ -758,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1018"/>
+  <dimension ref="A1:Z1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -872,7 +887,7 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -1078,7 +1093,7 @@
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>68</v>
@@ -1086,10 +1101,10 @@
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
@@ -1098,7 +1113,7 @@
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>68</v>
@@ -1106,10 +1121,10 @@
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
@@ -1118,18 +1133,18 @@
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" s="5" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
@@ -1138,18 +1153,18 @@
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1">
@@ -1158,27 +1173,48 @@
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1">
       <c r="A54" s="5" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-    </row>
-    <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="A57" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A58" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+    </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2137,6 +2173,9 @@
     <row r="1016" ht="14.25" customHeight="1"/>
     <row r="1017" ht="14.25" customHeight="1"/>
     <row r="1018" ht="14.25" customHeight="1"/>
+    <row r="1019" ht="14.25" customHeight="1"/>
+    <row r="1020" ht="14.25" customHeight="1"/>
+    <row r="1021" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated Loop brief for validation
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6360F44-EC36-42AE-B223-BD9B06762DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5B4CC8-2A75-41E3-8692-4789DC849CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,13 +234,6 @@
   </si>
   <si>
     <t>Hi Team,
-Found System Exception for the Document: {0}. Please check Below for the Exception Message.
-System Exception:{1}
-Thanks,
-Digital User.</t>
-  </si>
-  <si>
-    <t>Hi Team,
 Attached you will find the summary report for documents which were processed by the system on {0}.
 Thanks,
 Digital User.</t>
@@ -388,6 +381,14 @@
   </si>
   <si>
     <t>People v. Delgadillo;Delgadillo</t>
+  </si>
+  <si>
+    <t>Hi Team,
+Found System Exception for the Document: {0}. Please check Below for the Exception Message.
+System Exception:
+{1}
+Thanks,
+Digital User.</t>
   </si>
 </sst>
 </file>
@@ -781,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -832,7 +833,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -843,7 +844,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -864,10 +865,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -885,7 +886,7 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -893,7 +894,7 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -939,7 +940,7 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>45</v>
@@ -947,40 +948,40 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="101.5">
       <c r="A24" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.5">
@@ -988,16 +989,16 @@
     </row>
     <row r="26" spans="1:3" ht="14.5">
       <c r="A26" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" ht="14.5">
       <c r="A27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>45</v>
@@ -1005,24 +1006,24 @@
     </row>
     <row r="28" spans="1:3" ht="14.5">
       <c r="A28" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:3" ht="14.5">
       <c r="A29" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="130.5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="145">
       <c r="A30" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.5">
@@ -1038,32 +1039,32 @@
     </row>
     <row r="33" spans="1:3" ht="87">
       <c r="A33" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.5">
       <c r="A34" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="14.5">
       <c r="A35" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.5">
       <c r="A36" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>45</v>
@@ -1071,16 +1072,16 @@
     </row>
     <row r="37" spans="1:3" ht="14.5">
       <c r="A37" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="14.5">
       <c r="A38" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
@@ -1101,7 +1102,7 @@
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>68</v>
@@ -1109,10 +1110,10 @@
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
@@ -1121,7 +1122,7 @@
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>68</v>
@@ -1129,10 +1130,10 @@
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
@@ -1141,7 +1142,7 @@
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>68</v>
@@ -1149,10 +1150,10 @@
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
@@ -1181,18 +1182,18 @@
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1">
       <c r="A54" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
@@ -1201,18 +1202,18 @@
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
       <c r="A57" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated with BRIEF - DELGADILLO BRIEF.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5B4CC8-2A75-41E3-8692-4789DC849CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22CD0C3-A08E-4F4D-B0D2-BB8E334A159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count,Declaration Regarding Word Count,Statement of Word Count,Certification of Compliance,Word Count@Statement of Appealability,Statement of Appellate Jurisdiction,Statement of Jurisdiction,Statement of Appelability,Appealability@Table of Contents,Topical Index@Table of Authorities,Table of Authority,Table of Cases and Authorities,Table of Cases@Statement of Facts,Statement of the Facts,Statement of the Case,Summary of Alleged Facts,Statements of Case and Procedural Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments@Declaration of Appellate Counsel,Declaration of Counsel,DECLARATION OF,COUNSEL DECLARATION,Certification of Appellate Counsel,Certificate of Appellate Counsel,Attest of Appellate Counsel,Attestation of Appellate Counsel</t>
-  </si>
-  <si>
-    <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count,Declaration Regarding Word Count,Statement of Word Count,Certification of Compliance,Word Count@Statement of Appealability,Statement of Appellate Jurisdiction,Statement of Jurisdiction,Statement of Appelability,Appealability@Table of Contents,Topical Index@Table of Authorities,Table of Authority,Table of Cases and Authorities,Table of Cases@Statement of Facts,Statement of the Facts,Statement of the Case,Summary of Alleged Facts,Statements of Case and Procedural Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments@Declaration of Appellate Counsel,Declaration of Counsel,DECLARATION OF,COUNSEL DECLARATION,Certification of Appellate Counsel,Certificate of Appellate Counsel,Attest of Appellate Counsel,Attestation of Appellate Counsel@court may treat the appeal as abandoned and dismiss the appeal,court may dismiss the appeal without issuing an opinion,may result in the court dismissing the appeal as abandoned,the appeal may be dismissed as abandoned,court very likely would dismiss the appeal as abandoned,no brief or letter is filed the appeal may be dismissed,court may treat the appeal as abandoned and dismiss,the court may dismiss the matter,the Court may dismiss the appeal as abandoned,if the appeal is dismissed as abandoned</t>
   </si>
   <si>
     <t>jgandikota@avereusa.com</t>
@@ -389,6 +386,15 @@
 {1}
 Thanks,
 Digital User.</t>
+  </si>
+  <si>
+    <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count,Declaration Regarding Word Count,Statement of Word Count,Certification of Compliance,Word Count@Statement of Appealability,Statement of Appellate Jurisdiction,Statement of Jurisdiction,Statement of Appelability,Appealability@Table of Contents,Topical Index@Table of Authorities,Table of Authority,Table of Cases and Authorities,Table of Cases@Statement of Facts,Statement of the Facts,Statement of the Case,Summary of Alleged Facts,Statements of Case and Procedural Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments@Declaration of Appellate Counsel,Declaration of Counsel,DECLARATION OF,COUNSEL DECLARATION,Certification of Appellate Counsel,Certificate of Appellate Counsel,Attest of Appellate Counsel,Attestation of Appellate Counsel@court may treat the appeal as abandoned and dismiss the appeal,court may dismiss the appeal without issuing an opinion,may result in the court dismissing the appeal as abandoned,the appeal may be dismissed as abandoned,court very likely would dismiss the appeal as abandoned,no brief or letter is filed the appeal may be dismissed,court may treat the appeal as abandoned and dismiss,the court may dismiss the matter,the Court may dismiss the appeal as abandoned,if the appeal is dismissed as abandoned,Court may treat his appeal as abandoned and dismiss,Court may treat her appeal as abandoned and dismiss,Court may treat their appeal as abandoned and dismiss,Court may treat they appeal as abandoned and dismiss</t>
+  </si>
+  <si>
+    <t>InputFolderPath</t>
+  </si>
+  <si>
+    <t>C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\Input\</t>
   </si>
 </sst>
 </file>
@@ -780,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1021"/>
+  <dimension ref="A1:Z1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -886,7 +892,7 @@
         <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -937,294 +943,301 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" t="s">
-        <v>113</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="101.5">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:3" ht="101.5">
+      <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.5">
-      <c r="B25" s="3"/>
-    </row>
     <row r="26" spans="1:3" ht="14.5">
-      <c r="A26" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="6"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:3" ht="14.5">
       <c r="A27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" ht="14.5">
       <c r="A28" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="14.5">
       <c r="A29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" ht="14.5">
+      <c r="A30" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="145">
-      <c r="A30" s="5" t="s">
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="145">
+      <c r="A31" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.5">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.5">
+      <c r="A32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.5">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" ht="87">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:3" ht="14.5">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" ht="87">
+      <c r="A34" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.5">
-      <c r="A34" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="14.5">
       <c r="A35" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>86</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" ht="14.5">
       <c r="A36" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.5">
       <c r="A37" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="14.5">
       <c r="A38" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:3" ht="14.5">
+      <c r="A39" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B38" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A41" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-    </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A44" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-    </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A45" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A47" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-    </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A48" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A50" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="B50" s="5" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A51" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A53" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B53" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-    </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A54" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>77</v>
-      </c>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
       <c r="A55" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A56" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-    </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A57" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A59" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="B59" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
     </row>
-    <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+    </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2185,6 +2198,7 @@
     <row r="1019" ht="14.25" customHeight="1"/>
     <row r="1020" ht="14.25" customHeight="1"/>
     <row r="1021" ht="14.25" customHeight="1"/>
+    <row r="1022" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First Commit for the RBF Brief Document
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22CD0C3-A08E-4F4D-B0D2-BB8E334A159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5432F19A-6A9F-4670-81EB-43C1503BECC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -113,9 +113,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
   </si>
   <si>
     <t>DocType</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
   </si>
   <si>
     <t>eric.wong-c@caljc.onmicrosoft.com</t>
@@ -329,9 +323,6 @@
     <t>3DCA Catalog</t>
   </si>
   <si>
-    <t>ActionCenterCatalog</t>
-  </si>
-  <si>
     <t>AOB_Citations</t>
   </si>
   <si>
@@ -354,9 +345,6 @@
   </si>
   <si>
     <t>Delgadillo_Headers</t>
-  </si>
-  <si>
-    <t>BRIEF - APPELLANT'S OPENING BRIEF;BRIEF - WENDE BRIEF;BRIEF - DELGADILLO BRIEF</t>
   </si>
   <si>
     <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count,Declaration Regarding Word Count,Statement of Word Count,Certification of Compliance,Word Count@Statement of Appealability,Statement of Appellate Jurisdiction,Statement of Jurisdiction,Statement of Appelability,Appealability@Table of Contents,Topical Index@Table of Authorities,Table of Authority,Table of Cases and Authorities,Table of Cases@Statement of Facts,Statement of the Facts,Statement of the Case,Summary of Alleged Facts,Statements of Case and Procedural Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments</t>
@@ -395,6 +383,51 @@
   </si>
   <si>
     <t>C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\Input\</t>
+  </si>
+  <si>
+    <t>BRIEF - APPELLANT'S OPENING BRIEF;BRIEF - WENDE BRIEF;BRIEF - DELGADILLO BRIEF;BRIEF - RESPONDENT'S BRIEF</t>
+  </si>
+  <si>
+    <t>Respondent_Headers</t>
+  </si>
+  <si>
+    <t>Respondent_Citations</t>
+  </si>
+  <si>
+    <t>Certificate of Compliance,Word Count Certification,Word Count Certificate,Certificate of Length,Certificate of Counsel,Certification of Word Count,Brief Format Certification,Certificate of Word Count,Declaration Regarding Word Count,Statement of Word Count,Certification of Compliance,Word Count@Table of Contents,Topical Index@Table of Authorities,Table of Authority,Table of Cases and Authorities,Table of Cases@Statement of Facts,Statement of the Facts,Statement of the Case,Summary of Alleged Facts,Statements of Case and Procedural Facts@Proof of Service,Certificate of Service,Proof of Service by Mail and Email,Proof of Service by Mail,Proof of Service by Mail/Electronic Service,Declaration of Service,Declaration of Service by Mail,Proof of Service by Mail and Electronically,Brief Format Certification Pursuant to California Rules of Court 8.360,Declaration of Electronic Service and Service by U.S. Mail,Attorney's Certificate of Electronic Service and Service by Mail,Attorney's Certificate of Service,@Argument,Arguments</t>
+  </si>
+  <si>
+    <t>BRIEF - RESPONDENT'S BRIEF</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder_Prod</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName_Prod</t>
+  </si>
+  <si>
+    <t>3DCA Queue</t>
+  </si>
+  <si>
+    <t>3DCA Sandbox</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName_Dev</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder_Dev</t>
+  </si>
+  <si>
+    <t>ActionCenterCatalog_Prod</t>
+  </si>
+  <si>
+    <t>ActionCenterCatalog_Dev</t>
+  </si>
+  <si>
+    <t>BucketPath_Prod</t>
+  </si>
+  <si>
+    <t>BucketPath_Dev</t>
   </si>
 </sst>
 </file>
@@ -786,16 +819,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1022"/>
+  <dimension ref="A1:Z1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.54296875" customWidth="1"/>
-    <col min="2" max="2" width="79.1796875" customWidth="1"/>
+    <col min="2" max="2" width="99.81640625" customWidth="1"/>
     <col min="3" max="3" width="81.453125" customWidth="1"/>
     <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
@@ -836,10 +869,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -847,287 +880,300 @@
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
-      <c r="A5" t="s">
+    </row>
+    <row r="4" spans="1:26" ht="14.5">
+      <c r="A4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.5">
+      <c r="A5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="29">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
-      </c>
-    </row>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-    </row>
+        <v>130</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>45</v>
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="87">
+      <c r="A30" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="101.5">
-      <c r="A25" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.5">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" ht="14.5">
-      <c r="A27" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" ht="14.5">
-      <c r="A28" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.5">
-      <c r="A29" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" ht="14.5">
-      <c r="A30" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="145">
-      <c r="A31" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>116</v>
-      </c>
+      <c r="B30" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.5">
+      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="14.5">
       <c r="A32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>65</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" ht="14.5">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:3" ht="87">
-      <c r="A34" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="A33" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.5">
+      <c r="A34" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="14.5">
       <c r="A35" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" ht="14.5">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="130.5">
       <c r="A36" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.5">
       <c r="A37" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>45</v>
+        <v>62</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.5">
-      <c r="A38" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="5"/>
-    </row>
-    <row r="39" spans="1:3" ht="14.5">
-      <c r="A39" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B39" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" ht="87">
+      <c r="A39" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.5">
+      <c r="A40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" ht="14.5">
       <c r="A41" s="5" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.5">
+      <c r="A42" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.5">
       <c r="A43" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+        <v>83</v>
+      </c>
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="1:3" ht="14.5">
       <c r="A44" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>109</v>
+        <v>95</v>
+      </c>
+      <c r="B44" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
@@ -1136,127 +1182,171 @@
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" s="5" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A47" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>110</v>
-      </c>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A50" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A53" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A56" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" s="5" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A59" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
+      <c r="A61" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+    </row>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A63" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A64" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A66" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A67" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+    </row>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>
     <row r="83" ht="14.25" customHeight="1"/>
@@ -2199,6 +2289,14 @@
     <row r="1020" ht="14.25" customHeight="1"/>
     <row r="1021" ht="14.25" customHeight="1"/>
     <row r="1022" ht="14.25" customHeight="1"/>
+    <row r="1023" ht="14.25" customHeight="1"/>
+    <row r="1024" ht="14.25" customHeight="1"/>
+    <row r="1025" ht="14.25" customHeight="1"/>
+    <row r="1026" ht="14.25" customHeight="1"/>
+    <row r="1027" ht="14.25" customHeight="1"/>
+    <row r="1028" ht="14.25" customHeight="1"/>
+    <row r="1029" ht="14.25" customHeight="1"/>
+    <row r="1030" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2269,13 +2367,13 @@
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2348,48 +2446,48 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3374,7 +3472,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3423,14 +3521,14 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>